<commit_message>
Thrive ASN expands now
</commit_message>
<xml_diff>
--- a/Finished/Thrive/Thrive ASN PO 304133 11.20.2024.xlsx
+++ b/Finished/Thrive/Thrive ASN PO 304133 11.20.2024.xlsx
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -320,6 +320,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -687,7 +690,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,10 +1225,8 @@
       </c>
     </row>
     <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="36" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A19" s="36" t="n">
+        <v>1</v>
       </c>
       <c r="B19" s="36" t="inlineStr">
         <is>
@@ -1240,29 +1241,23 @@
       <c r="D19" s="22" t="n"/>
       <c r="E19" s="36" t="inlineStr">
         <is>
+          <t>850016364852</t>
+        </is>
+      </c>
+      <c r="F19" s="36" t="inlineStr">
+        <is>
           <t>Edi-STRESS-PB-L</t>
         </is>
       </c>
-      <c r="F19" s="36" t="inlineStr">
-        <is>
-          <t>850016364852</t>
-        </is>
-      </c>
-      <c r="G19" s="36" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="G19" s="36" t="n">
+        <v>1</v>
       </c>
       <c r="H19" s="36" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="I19" s="36" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="I19" s="22" t="n"/>
       <c r="J19" s="36" t="inlineStr">
         <is>
           <t>Stress Releaf, Peanut Butter C</t>
@@ -1272,10 +1267,8 @@
       <c r="L19" s="23" t="n"/>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="36" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A20" s="36" t="n">
+        <v>2</v>
       </c>
       <c r="B20" s="36" t="inlineStr">
         <is>
@@ -1290,29 +1283,23 @@
       <c r="D20" s="22" t="n"/>
       <c r="E20" s="36" t="inlineStr">
         <is>
+          <t>850016364883</t>
+        </is>
+      </c>
+      <c r="F20" s="36" t="inlineStr">
+        <is>
           <t>Edi-HJ-PB-LRG</t>
         </is>
       </c>
-      <c r="F20" s="36" t="inlineStr">
-        <is>
-          <t>850016364883</t>
-        </is>
-      </c>
-      <c r="G20" s="36" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G20" s="36" t="n">
+        <v>4</v>
       </c>
       <c r="H20" s="36" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="I20" s="36" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
+      <c r="I20" s="22" t="n"/>
       <c r="J20" s="36" t="inlineStr">
         <is>
           <t>Hip &amp; Joint Releaf, Peanut But</t>
@@ -1322,10 +1309,8 @@
       <c r="L20" s="23" t="n"/>
     </row>
     <row r="21" ht="18.75" customHeight="1">
-      <c r="A21" s="36" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A21" s="36" t="n">
+        <v>3</v>
       </c>
       <c r="B21" s="36" t="inlineStr">
         <is>
@@ -1340,50 +1325,642 @@
       <c r="D21" s="22" t="n"/>
       <c r="E21" s="36" t="inlineStr">
         <is>
-          <t>2in1-SK-CT</t>
+          <t>850016364883</t>
         </is>
       </c>
       <c r="F21" s="36" t="inlineStr">
         <is>
-          <t>860008876744</t>
-        </is>
-      </c>
-      <c r="G21" s="36" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+          <t>Edi-HJ-PB-LRG</t>
+        </is>
+      </c>
+      <c r="G21" s="36" t="n">
+        <v>4</v>
       </c>
       <c r="H21" s="36" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="I21" s="36" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+      <c r="I21" s="22" t="n"/>
       <c r="J21" s="36" t="inlineStr">
         <is>
-          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+          <t>Hip &amp; Joint Releaf, Peanut But</t>
         </is>
       </c>
       <c r="K21" s="23" t="n"/>
       <c r="L21" s="23" t="n"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="24" t="n"/>
-      <c r="B22" s="23" t="n"/>
-      <c r="C22" s="23" t="n"/>
+      <c r="A22" s="36" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="36" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C22" s="36" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
       <c r="D22" s="23" t="n"/>
-      <c r="E22" s="23" t="n"/>
-      <c r="F22" s="23" t="n"/>
-      <c r="G22" s="22" t="n"/>
-      <c r="H22" s="23" t="n"/>
+      <c r="E22" s="36" t="inlineStr">
+        <is>
+          <t>850016364883</t>
+        </is>
+      </c>
+      <c r="F22" s="36" t="inlineStr">
+        <is>
+          <t>Edi-HJ-PB-LRG</t>
+        </is>
+      </c>
+      <c r="G22" s="36" t="n">
+        <v>4</v>
+      </c>
+      <c r="H22" s="36" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
       <c r="I22" s="23" t="n"/>
-      <c r="J22" s="23" t="n"/>
+      <c r="J22" s="36" t="inlineStr">
+        <is>
+          <t>Hip &amp; Joint Releaf, Peanut But</t>
+        </is>
+      </c>
       <c r="K22" s="23" t="n"/>
       <c r="L22" s="23" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="37" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C23" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E23" s="37" t="inlineStr">
+        <is>
+          <t>850016364883</t>
+        </is>
+      </c>
+      <c r="F23" s="37" t="inlineStr">
+        <is>
+          <t>Edi-HJ-PB-LRG</t>
+        </is>
+      </c>
+      <c r="G23" s="37" t="n">
+        <v>4</v>
+      </c>
+      <c r="H23" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J23" s="37" t="inlineStr">
+        <is>
+          <t>Hip &amp; Joint Releaf, Peanut But</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="37" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C24" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E24" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F24" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G24" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H24" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J24" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="37" t="n">
+        <v>7</v>
+      </c>
+      <c r="B25" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C25" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E25" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F25" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G25" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H25" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J25" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="37" t="n">
+        <v>8</v>
+      </c>
+      <c r="B26" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C26" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E26" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F26" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G26" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H26" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J26" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="37" t="n">
+        <v>9</v>
+      </c>
+      <c r="B27" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C27" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E27" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F27" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G27" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H27" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J27" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="37" t="n">
+        <v>10</v>
+      </c>
+      <c r="B28" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C28" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E28" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F28" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G28" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H28" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J28" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="37" t="n">
+        <v>11</v>
+      </c>
+      <c r="B29" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C29" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E29" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F29" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G29" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H29" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J29" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="37" t="n">
+        <v>12</v>
+      </c>
+      <c r="B30" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C30" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E30" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F30" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G30" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H30" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J30" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="37" t="n">
+        <v>13</v>
+      </c>
+      <c r="B31" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C31" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E31" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F31" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G31" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H31" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J31" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="B32" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C32" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E32" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F32" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G32" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H32" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J32" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="37" t="n">
+        <v>15</v>
+      </c>
+      <c r="B33" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C33" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E33" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F33" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G33" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H33" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J33" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="37" t="n">
+        <v>16</v>
+      </c>
+      <c r="B34" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C34" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E34" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F34" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G34" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H34" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J34" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="37" t="n">
+        <v>17</v>
+      </c>
+      <c r="B35" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C35" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E35" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F35" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G35" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H35" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J35" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="37" t="n">
+        <v>18</v>
+      </c>
+      <c r="B36" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C36" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E36" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F36" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G36" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H36" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J36" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="37" t="n">
+        <v>19</v>
+      </c>
+      <c r="B37" s="37" t="inlineStr">
+        <is>
+          <t>304133</t>
+        </is>
+      </c>
+      <c r="C37" s="37" t="inlineStr">
+        <is>
+          <t>10/15/2024</t>
+        </is>
+      </c>
+      <c r="E37" s="37" t="inlineStr">
+        <is>
+          <t>860008876744</t>
+        </is>
+      </c>
+      <c r="F37" s="37" t="inlineStr">
+        <is>
+          <t>2in1-SK-CT</t>
+        </is>
+      </c>
+      <c r="G37" s="37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H37" s="37" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="J37" s="37" t="inlineStr">
+        <is>
+          <t>Skin &amp; Coat Releaf 100mg CBD 2</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>